<commit_message>
Update source SITs and unit_counters.json for GOR, HYD, KLI, KZI.
</commit_message>
<xml_diff>
--- a/sits/msit_gorns.xlsx
+++ b/sits/msit_gorns.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="829">
   <si>
     <t>Designation</t>
   </si>
@@ -2295,6 +2295,9 @@
       </rPr>
       <t xml:space="preserve">/None</t>
     </r>
+  </si>
+  <si>
+    <t>Y182F</t>
   </si>
   <si>
     <t>PF Tender Pod, limit 2; Scout; (2EW:2AF)(1EW:TugAF)</t>
@@ -3875,7 +3878,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
@@ -3888,13 +3891,6 @@
       <right style="thick"/>
       <top style="thick"/>
       <bottom style="thick"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
       <diagonal/>
     </border>
   </borders>
@@ -3923,7 +3919,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="39">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -4068,26 +4064,6 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="6" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
@@ -4179,8 +4155,8 @@
   </sheetPr>
   <dimension ref="A1:K197"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A167" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A169" activeCellId="0" pane="topLeft" sqref="169:170"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A106" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G119" activeCellId="0" pane="topLeft" sqref="G119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7861,7 +7837,7 @@
         <v>505</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="E116" s="20" t="n">
         <v>2</v>
@@ -7966,13 +7942,13 @@
         <v>515</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="E119" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>155</v>
+        <v>516</v>
       </c>
       <c r="G119" s="24" t="s">
         <v>507</v>
@@ -7987,18 +7963,18 @@
         <v>0.5</v>
       </c>
       <c r="K119" s="9" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="120">
       <c r="A120" s="5" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B120" s="6" t="n">
         <v>99</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>64</v>
@@ -8016,24 +7992,24 @@
         <v>17</v>
       </c>
       <c r="I120" s="5" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="J120" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="K120" s="9" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="121">
       <c r="A121" s="5" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B121" s="6" t="n">
         <v>97</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>64</v>
@@ -8042,7 +8018,7 @@
         <v>1</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="G121" s="24" t="s">
         <v>507</v>
@@ -8051,24 +8027,24 @@
         <v>17</v>
       </c>
       <c r="I121" s="5" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="J121" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="K121" s="9" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="122">
       <c r="A122" s="9" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B122" s="22" t="n">
         <v>7</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>58</v>
@@ -8077,7 +8053,7 @@
         <v>0</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="G122" s="21" t="s">
         <v>507</v>
@@ -8086,24 +8062,24 @@
         <v>17</v>
       </c>
       <c r="I122" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="J122" s="23" t="n">
         <v>0.5</v>
       </c>
       <c r="K122" s="9" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="123">
       <c r="A123" s="9" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B123" s="20" t="n">
         <v>98</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>64</v>
@@ -8121,24 +8097,24 @@
         <v>17</v>
       </c>
       <c r="I123" s="9" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="J123" s="23" t="n">
         <v>0.5</v>
       </c>
       <c r="K123" s="9" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="124">
       <c r="A124" s="9" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B124" s="21" t="s">
         <v>50</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D124" s="9" t="s">
         <v>32</v>
@@ -8147,27 +8123,27 @@
         <v>0</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="G124" s="9" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="H124" s="9" t="s">
         <v>480</v>
       </c>
       <c r="I124" s="9" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="J124" s="23" t="n">
         <v>0</v>
       </c>
       <c r="K124" s="9" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="125">
       <c r="A125" s="3" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -8182,13 +8158,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="126">
       <c r="A126" s="9" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>64</v>
@@ -8197,7 +8173,7 @@
         <v>0</v>
       </c>
       <c r="F126" s="9" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="G126" s="9" t="s">
         <v>480</v>
@@ -8206,21 +8182,21 @@
         <v>480</v>
       </c>
       <c r="I126" s="9" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="J126" s="23" t="n">
         <v>0</v>
       </c>
       <c r="K126" s="9" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="127">
       <c r="A127" s="9" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C127" s="21" t="s">
         <v>17</v>
@@ -8232,7 +8208,7 @@
         <v>0</v>
       </c>
       <c r="F127" s="9" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="G127" s="9" t="s">
         <v>480</v>
@@ -8241,18 +8217,18 @@
         <v>480</v>
       </c>
       <c r="I127" s="9" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="J127" s="23" t="n">
         <v>0</v>
       </c>
       <c r="K127" s="9" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="128">
       <c r="A128" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -8267,13 +8243,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="129">
       <c r="A129" s="9" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D129" s="9" t="s">
         <v>58</v>
@@ -8282,33 +8258,33 @@
         <v>6</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="G129" s="9" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="H129" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I129" s="9" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="J129" s="23" t="n">
         <v>2</v>
       </c>
       <c r="K129" s="9" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="130">
       <c r="A130" s="5" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D130" s="5" t="s">
         <v>58</v>
@@ -8320,30 +8296,30 @@
         <v>152</v>
       </c>
       <c r="G130" s="9" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="H130" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I130" s="5" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="J130" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="K130" s="5" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="131">
       <c r="A131" s="5" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>485</v>
@@ -8355,30 +8331,30 @@
         <v>200</v>
       </c>
       <c r="G131" s="9" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="H131" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I131" s="5" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="J131" s="29" t="n">
         <v>0</v>
       </c>
       <c r="K131" s="5" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="132">
       <c r="A132" s="9" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>58</v>
@@ -8390,24 +8366,24 @@
         <v>200</v>
       </c>
       <c r="G132" s="9" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="H132" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I132" s="5" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="J132" s="10" t="n">
         <v>1</v>
       </c>
       <c r="K132" s="5" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="133">
       <c r="A133" s="3" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -8422,7 +8398,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="134">
       <c r="A134" s="9" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
@@ -8437,7 +8413,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="135">
       <c r="A135" s="3" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -8452,13 +8428,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="136">
       <c r="A136" s="9" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D136" s="9" t="s">
         <v>58</v>
@@ -8470,33 +8446,33 @@
         <v>127</v>
       </c>
       <c r="G136" s="9" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H136" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I136" s="9" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="J136" s="23" t="n">
         <v>1</v>
       </c>
       <c r="K136" s="9" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="137">
       <c r="A137" s="5" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="E137" s="8" t="n">
         <v>6</v>
@@ -8505,30 +8481,30 @@
         <v>336</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H137" s="5" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="I137" s="5" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="J137" s="10" t="n">
         <v>1</v>
       </c>
       <c r="K137" s="9" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="138">
       <c r="A138" s="5" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="D138" s="5" t="s">
         <v>64</v>
@@ -8540,30 +8516,30 @@
         <v>200</v>
       </c>
       <c r="G138" s="5" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H138" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I138" s="5" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="J138" s="10" t="n">
         <v>1</v>
       </c>
       <c r="K138" s="9" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="139">
       <c r="A139" s="9" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D139" s="9" t="s">
         <v>64</v>
@@ -8572,33 +8548,33 @@
         <v>0</v>
       </c>
       <c r="F139" s="9" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="G139" s="9" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H139" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I139" s="9" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="J139" s="23" t="n">
         <v>1</v>
       </c>
       <c r="K139" s="9" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="140">
       <c r="A140" s="5" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D140" s="5" t="s">
         <v>58</v>
@@ -8607,33 +8583,33 @@
         <v>6</v>
       </c>
       <c r="F140" s="5" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="G140" s="5" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H140" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I140" s="5" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="J140" s="10" t="n">
         <v>1</v>
       </c>
       <c r="K140" s="5" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="141">
       <c r="A141" s="9" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B141" s="20" t="n">
         <v>25</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D141" s="9" t="s">
         <v>32</v>
@@ -8642,33 +8618,33 @@
         <v>0</v>
       </c>
       <c r="F141" s="9" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="G141" s="9" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H141" s="9" t="s">
         <v>480</v>
       </c>
       <c r="I141" s="9" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="J141" s="23" t="n">
         <v>0</v>
       </c>
       <c r="K141" s="9" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="142">
       <c r="A142" s="5" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="C142" s="30" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="D142" s="5" t="s">
         <v>64</v>
@@ -8680,30 +8656,30 @@
         <v>200</v>
       </c>
       <c r="G142" s="5" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H142" s="9" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="I142" s="5" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="J142" s="10" t="n">
         <v>1</v>
       </c>
       <c r="K142" s="5" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="143">
       <c r="A143" s="9" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D143" s="9" t="s">
         <v>172</v>
@@ -8715,24 +8691,24 @@
         <v>127</v>
       </c>
       <c r="G143" s="9" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="H143" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I143" s="9" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="J143" s="23" t="n">
         <v>1</v>
       </c>
       <c r="K143" s="9" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="144">
       <c r="A144" s="3" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
@@ -8747,13 +8723,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="145">
       <c r="A145" s="9" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B145" s="20" t="n">
         <v>18</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D145" s="9" t="s">
         <v>58</v>
@@ -8765,33 +8741,33 @@
         <v>127</v>
       </c>
       <c r="G145" s="9" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="H145" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I145" s="9" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="J145" s="23" t="n">
         <v>0.5</v>
       </c>
       <c r="K145" s="9" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="146">
       <c r="A146" s="5" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="E146" s="8" t="n">
         <v>3</v>
@@ -8800,19 +8776,19 @@
         <v>336</v>
       </c>
       <c r="G146" s="5" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="H146" s="5" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="I146" s="5" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="J146" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="K146" s="9" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="147">
@@ -8852,13 +8828,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="148">
       <c r="A148" s="5" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>64</v>
@@ -8870,30 +8846,30 @@
         <v>200</v>
       </c>
       <c r="G148" s="5" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="H148" s="5" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="I148" s="5" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="J148" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="K148" s="9" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="149">
       <c r="A149" s="9" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="D149" s="9" t="s">
         <v>64</v>
@@ -8902,33 +8878,33 @@
         <v>0</v>
       </c>
       <c r="F149" s="9" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="G149" s="9" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="H149" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I149" s="9" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="J149" s="23" t="n">
         <v>0.5</v>
       </c>
       <c r="K149" s="9" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="150">
       <c r="A150" s="5" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D150" s="5" t="s">
         <v>58</v>
@@ -8940,24 +8916,24 @@
         <v>152</v>
       </c>
       <c r="G150" s="5" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="H150" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I150" s="5" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="J150" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="K150" s="5" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="151">
       <c r="A151" s="3" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
@@ -8972,13 +8948,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="152">
       <c r="A152" s="9" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B152" s="22" t="n">
         <v>5</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="D152" s="9" t="s">
         <v>32</v>
@@ -8996,24 +8972,24 @@
         <v>480</v>
       </c>
       <c r="I152" s="9" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="J152" s="23" t="n">
         <v>0</v>
       </c>
       <c r="K152" s="9" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="153">
       <c r="A153" s="5" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>172</v>
@@ -9025,30 +9001,30 @@
         <v>478</v>
       </c>
       <c r="G153" s="5" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="H153" s="24" t="s">
         <v>17</v>
       </c>
       <c r="I153" s="5" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="J153" s="10" t="n">
         <v>0.2</v>
       </c>
       <c r="K153" s="9" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="154">
       <c r="A154" s="5" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B154" s="6" t="n">
         <v>67</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="D154" s="5" t="s">
         <v>172</v>
@@ -9057,33 +9033,33 @@
         <v>3</v>
       </c>
       <c r="F154" s="5" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="G154" s="5" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="H154" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I154" s="5" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="J154" s="29" t="n">
         <v>0</v>
       </c>
       <c r="K154" s="9" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="155">
       <c r="A155" s="9" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="D155" s="5" t="s">
         <v>58</v>
@@ -9101,24 +9077,24 @@
         <v>17</v>
       </c>
       <c r="I155" s="9" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="J155" s="10" t="n">
         <v>0</v>
       </c>
       <c r="K155" s="5" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="156">
       <c r="A156" s="5" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="D156" s="5" t="s">
         <v>58</v>
@@ -9133,27 +9109,27 @@
         <v>52</v>
       </c>
       <c r="H156" s="9" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="I156" s="5" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="J156" s="10" t="n">
         <v>0</v>
       </c>
       <c r="K156" s="5" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="157">
       <c r="A157" s="25" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B157" s="26" t="n">
         <v>45</v>
       </c>
       <c r="C157" s="35" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D157" s="25" t="s">
         <v>172</v>
@@ -9165,30 +9141,30 @@
         <v>40</v>
       </c>
       <c r="G157" s="25" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="H157" s="25" t="s">
         <v>17</v>
       </c>
       <c r="I157" s="25" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="J157" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K157" s="9" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="158">
       <c r="A158" s="5" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>172</v>
@@ -9212,18 +9188,18 @@
         <v>0</v>
       </c>
       <c r="K158" s="9" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="159">
       <c r="A159" s="9" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B159" s="20" t="n">
         <v>20</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="D159" s="9" t="s">
         <v>64</v>
@@ -9241,24 +9217,24 @@
         <v>17</v>
       </c>
       <c r="I159" s="9" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="J159" s="23" t="n">
         <v>0</v>
       </c>
       <c r="K159" s="9" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="160">
       <c r="A160" s="5" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B160" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="C160" s="5" t="s">
         <v>683</v>
-      </c>
-      <c r="C160" s="5" t="s">
-        <v>682</v>
       </c>
       <c r="D160" s="5" t="s">
         <v>58</v>
@@ -9276,18 +9252,18 @@
         <v>480</v>
       </c>
       <c r="I160" s="5" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="J160" s="29" t="n">
         <v>0</v>
       </c>
       <c r="K160" s="5" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="161">
       <c r="A161" s="3" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B161" s="3"/>
       <c r="C161" s="4"/>
@@ -9302,13 +9278,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="162">
       <c r="A162" s="9" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="D162" s="9" t="s">
         <v>32</v>
@@ -9320,30 +9296,30 @@
         <v>142</v>
       </c>
       <c r="G162" s="9" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="H162" s="9" t="s">
         <v>480</v>
       </c>
       <c r="I162" s="9" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="J162" s="23" t="n">
         <v>0</v>
       </c>
       <c r="K162" s="9" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="163">
       <c r="A163" s="9" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="D163" s="9" t="s">
         <v>64</v>
@@ -9352,33 +9328,33 @@
         <v>0</v>
       </c>
       <c r="F163" s="9" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="G163" s="9" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="H163" s="9" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="I163" s="9" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="J163" s="23" t="n">
         <v>0</v>
       </c>
       <c r="K163" s="9" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="164">
       <c r="A164" s="5" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D164" s="5" t="s">
         <v>64</v>
@@ -9390,30 +9366,30 @@
         <v>155</v>
       </c>
       <c r="G164" s="5" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="H164" s="5" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="I164" s="5" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="J164" s="10" t="n">
         <v>0</v>
       </c>
       <c r="K164" s="5" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="165">
       <c r="A165" s="5" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="D165" s="5" t="s">
         <v>485</v>
@@ -9431,18 +9407,18 @@
         <v>480</v>
       </c>
       <c r="I165" s="5" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="J165" s="29" t="n">
         <v>0</v>
       </c>
       <c r="K165" s="5" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="166">
       <c r="A166" s="3" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
@@ -9457,13 +9433,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="167">
       <c r="A167" s="25" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B167" s="25" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C167" s="30" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="D167" s="25" t="s">
         <v>58</v>
@@ -9475,30 +9451,30 @@
         <v>127</v>
       </c>
       <c r="G167" s="25" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="H167" s="9" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="I167" s="25" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="J167" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K167" s="9" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="168">
       <c r="A168" s="5" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="C168" s="30" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="D168" s="5" t="s">
         <v>32</v>
@@ -9507,103 +9483,103 @@
         <v>9</v>
       </c>
       <c r="F168" s="5" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="G168" s="5" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="H168" s="9" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="I168" s="5" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="J168" s="29" t="n">
         <v>0</v>
       </c>
       <c r="K168" s="9" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="169">
-      <c r="A169" s="36" t="s">
-        <v>721</v>
-      </c>
-      <c r="B169" s="37" t="n">
+      <c r="A169" s="9" t="s">
+        <v>722</v>
+      </c>
+      <c r="B169" s="20" t="n">
         <v>24</v>
       </c>
-      <c r="C169" s="38" t="s">
-        <v>536</v>
-      </c>
-      <c r="D169" s="36" t="s">
+      <c r="C169" s="31" t="s">
+        <v>537</v>
+      </c>
+      <c r="D169" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E169" s="39" t="n">
+      <c r="E169" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F169" s="36" t="s">
+      <c r="F169" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="G169" s="36" t="s">
-        <v>722</v>
-      </c>
-      <c r="H169" s="36" t="s">
+      <c r="G169" s="9" t="s">
+        <v>723</v>
+      </c>
+      <c r="H169" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="I169" s="36" t="s">
-        <v>690</v>
-      </c>
-      <c r="J169" s="40" t="n">
+      <c r="I169" s="9" t="s">
+        <v>691</v>
+      </c>
+      <c r="J169" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="K169" s="36" t="s">
+      <c r="K169" s="9" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="170">
+      <c r="A170" s="9" t="s">
+        <v>725</v>
+      </c>
+      <c r="B170" s="20" t="n">
+        <v>24</v>
+      </c>
+      <c r="C170" s="31" t="s">
+        <v>726</v>
+      </c>
+      <c r="D170" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E170" s="22" t="n">
+        <v>6</v>
+      </c>
+      <c r="F170" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G170" s="9" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="170">
-      <c r="A170" s="36" t="s">
-        <v>724</v>
-      </c>
-      <c r="B170" s="37" t="n">
-        <v>24</v>
-      </c>
-      <c r="C170" s="38" t="s">
-        <v>725</v>
-      </c>
-      <c r="D170" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="E170" s="39" t="n">
-        <v>6</v>
-      </c>
-      <c r="F170" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="G170" s="36" t="s">
-        <v>722</v>
-      </c>
-      <c r="H170" s="36" t="s">
+      <c r="H170" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="I170" s="36" t="s">
+      <c r="I170" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="J170" s="40" t="n">
+      <c r="J170" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="K170" s="36" t="s">
-        <v>726</v>
+      <c r="K170" s="9" t="s">
+        <v>727</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="171">
       <c r="A171" s="5" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C171" s="31" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="D171" s="5" t="s">
         <v>32</v>
@@ -9612,33 +9588,33 @@
         <v>10</v>
       </c>
       <c r="F171" s="5" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="G171" s="5" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="H171" s="5" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="I171" s="5" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="J171" s="29" t="n">
         <v>0</v>
       </c>
       <c r="K171" s="9" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="172">
       <c r="A172" s="9" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B172" s="8" t="n">
         <v>4</v>
       </c>
       <c r="C172" s="30" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="D172" s="5" t="s">
         <v>32</v>
@@ -9647,7 +9623,7 @@
         <v>0</v>
       </c>
       <c r="F172" s="5" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="G172" s="5" t="s">
         <v>480</v>
@@ -9656,24 +9632,24 @@
         <v>480</v>
       </c>
       <c r="I172" s="5" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="J172" s="10" t="n">
         <v>0</v>
       </c>
       <c r="K172" s="5" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="173">
       <c r="A173" s="9" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C173" s="21" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="D173" s="9" t="s">
         <v>39</v>
@@ -9691,24 +9667,24 @@
         <v>480</v>
       </c>
       <c r="I173" s="9" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="J173" s="23" t="n">
         <v>0</v>
       </c>
       <c r="K173" s="9" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="174">
       <c r="A174" s="5" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C174" s="7" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="D174" s="5" t="s">
         <v>172</v>
@@ -9720,33 +9696,33 @@
         <v>40</v>
       </c>
       <c r="G174" s="5" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H174" s="9" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="I174" s="5" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="J174" s="29" t="n">
         <v>0</v>
       </c>
       <c r="K174" s="9" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="175">
       <c r="A175" s="25" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C175" s="30" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="D175" s="25" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="E175" s="27" t="n">
         <v>9</v>
@@ -9755,30 +9731,30 @@
         <v>155</v>
       </c>
       <c r="G175" s="25" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="H175" s="5" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="I175" s="25" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="J175" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K175" s="9" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="176">
       <c r="A176" s="25" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="C176" s="30" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="D176" s="25" t="s">
         <v>64</v>
@@ -9790,30 +9766,30 @@
         <v>155</v>
       </c>
       <c r="G176" s="25" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="H176" s="9" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="I176" s="25" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="J176" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K176" s="9" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="177">
       <c r="A177" s="25" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B177" s="25" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C177" s="35" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="D177" s="25" t="s">
         <v>64</v>
@@ -9825,30 +9801,30 @@
         <v>155</v>
       </c>
       <c r="G177" s="25" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="H177" s="9" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="I177" s="25" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="J177" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K177" s="9" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="178">
       <c r="A178" s="9" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B178" s="6" t="n">
         <v>16</v>
       </c>
       <c r="C178" s="24" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="D178" s="5" t="s">
         <v>64</v>
@@ -9866,24 +9842,24 @@
         <v>480</v>
       </c>
       <c r="I178" s="5" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="J178" s="29" t="n">
         <v>0</v>
       </c>
       <c r="K178" s="5" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="179">
       <c r="A179" s="9" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B179" s="26" t="n">
         <v>17</v>
       </c>
-      <c r="C179" s="41" t="s">
-        <v>768</v>
+      <c r="C179" s="36" t="s">
+        <v>769</v>
       </c>
       <c r="D179" s="25" t="s">
         <v>64</v>
@@ -9901,24 +9877,24 @@
         <v>480</v>
       </c>
       <c r="I179" s="25" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="J179" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K179" s="5" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="180">
       <c r="A180" s="25" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C180" s="30" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="D180" s="25" t="s">
         <v>172</v>
@@ -9930,30 +9906,30 @@
         <v>59</v>
       </c>
       <c r="G180" s="25" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H180" s="9" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="I180" s="25" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="J180" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K180" s="9" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="181">
       <c r="A181" s="16" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B181" s="16" t="s">
-        <v>777</v>
-      </c>
-      <c r="C181" s="42" t="s">
         <v>778</v>
+      </c>
+      <c r="C181" s="37" t="s">
+        <v>779</v>
       </c>
       <c r="D181" s="16" t="s">
         <v>473</v>
@@ -9965,24 +9941,24 @@
         <v>109</v>
       </c>
       <c r="G181" s="16" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="H181" s="11" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="I181" s="16" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="J181" s="34" t="n">
         <v>0</v>
       </c>
       <c r="K181" s="11" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="182">
       <c r="A182" s="3" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
@@ -9997,13 +9973,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="183">
       <c r="A183" s="5" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="D183" s="5" t="s">
         <v>64</v>
@@ -10021,24 +9997,24 @@
         <v>480</v>
       </c>
       <c r="I183" s="9" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="J183" s="10" t="n">
         <v>0</v>
       </c>
       <c r="K183" s="5" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="184">
       <c r="A184" s="5" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="D184" s="5" t="s">
         <v>32</v>
@@ -10053,27 +10029,27 @@
         <v>480</v>
       </c>
       <c r="H184" s="5" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="I184" s="9" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="J184" s="10" t="n">
         <v>0</v>
       </c>
       <c r="K184" s="5" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="185">
       <c r="A185" s="9" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>485</v>
@@ -10088,16 +10064,16 @@
         <v>480</v>
       </c>
       <c r="H185" s="9" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="I185" s="9" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="J185" s="32" t="n">
         <v>0</v>
       </c>
       <c r="K185" s="9" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="186">
@@ -10137,13 +10113,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="187">
       <c r="A187" s="9" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C187" s="9" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D187" s="9" t="s">
         <v>485</v>
@@ -10161,24 +10137,24 @@
         <v>480</v>
       </c>
       <c r="I187" s="9" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="J187" s="32" t="n">
         <v>0</v>
       </c>
       <c r="K187" s="9" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="188">
       <c r="A188" s="5" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D188" s="5" t="s">
         <v>485</v>
@@ -10196,18 +10172,18 @@
         <v>480</v>
       </c>
       <c r="I188" s="5" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="J188" s="29" t="n">
         <v>0</v>
       </c>
       <c r="K188" s="5" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="189">
       <c r="A189" s="3" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
@@ -10235,13 +10211,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="191">
       <c r="A191" s="5" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C191" s="24" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D191" s="5" t="s">
         <v>172</v>
@@ -10250,7 +10226,7 @@
         <v>0</v>
       </c>
       <c r="F191" s="5" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="G191" s="5" t="s">
         <v>480</v>
@@ -10259,24 +10235,24 @@
         <v>480</v>
       </c>
       <c r="I191" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="J191" s="10" t="n">
         <v>0</v>
       </c>
       <c r="K191" s="5" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="192">
       <c r="A192" s="5" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C192" s="21" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="D192" s="5" t="s">
         <v>485</v>
@@ -10285,7 +10261,7 @@
         <v>1</v>
       </c>
       <c r="F192" s="9" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="G192" s="5" t="s">
         <v>480</v>
@@ -10294,24 +10270,24 @@
         <v>480</v>
       </c>
       <c r="I192" s="5" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="J192" s="29" t="n">
         <v>0</v>
       </c>
       <c r="K192" s="5" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="193">
       <c r="A193" s="9" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="D193" s="9" t="s">
         <v>485</v>
@@ -10320,7 +10296,7 @@
         <v>0</v>
       </c>
       <c r="F193" s="9" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="G193" s="9" t="s">
         <v>480</v>
@@ -10329,24 +10305,24 @@
         <v>480</v>
       </c>
       <c r="I193" s="9" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="J193" s="32" t="n">
         <v>0</v>
       </c>
       <c r="K193" s="9" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="194">
       <c r="A194" s="9" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C194" s="9" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="D194" s="9" t="s">
         <v>485</v>
@@ -10355,7 +10331,7 @@
         <v>0</v>
       </c>
       <c r="F194" s="9" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="G194" s="9" t="s">
         <v>480</v>
@@ -10364,24 +10340,24 @@
         <v>480</v>
       </c>
       <c r="I194" s="9" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="J194" s="32" t="n">
         <v>0</v>
       </c>
       <c r="K194" s="9" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="195">
       <c r="A195" s="7" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C195" s="7" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>64</v>
@@ -10399,33 +10375,33 @@
         <v>480</v>
       </c>
       <c r="I195" s="9" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="J195" s="23" t="n">
         <v>0</v>
       </c>
       <c r="K195" s="9" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="196">
-      <c r="A196" s="43" t="s">
-        <v>826</v>
-      </c>
-      <c r="B196" s="43"/>
-      <c r="C196" s="43"/>
-      <c r="D196" s="43"/>
-      <c r="E196" s="43"/>
-      <c r="F196" s="43"/>
-      <c r="G196" s="43"/>
-      <c r="H196" s="43"/>
-      <c r="I196" s="43"/>
-      <c r="J196" s="43"/>
-      <c r="K196" s="43"/>
+      <c r="A196" s="38" t="s">
+        <v>827</v>
+      </c>
+      <c r="B196" s="38"/>
+      <c r="C196" s="38"/>
+      <c r="D196" s="38"/>
+      <c r="E196" s="38"/>
+      <c r="F196" s="38"/>
+      <c r="G196" s="38"/>
+      <c r="H196" s="38"/>
+      <c r="I196" s="38"/>
+      <c r="J196" s="38"/>
+      <c r="K196" s="38"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="197">
       <c r="A197" s="11" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B197" s="11"/>
       <c r="C197" s="11"/>

</xml_diff>

<commit_message>
Removed FTM from GOR source SIT.
</commit_message>
<xml_diff>
--- a/sits/msit_gorns.xlsx
+++ b/sits/msit_gorns.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="830">
   <si>
     <t>Designation</t>
   </si>
@@ -3233,6 +3233,9 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
+  </si>
+  <si>
+    <t>F&amp;E (WTF?)</t>
   </si>
   <si>
     <t>(441.4): 1+3</t>
@@ -4155,8 +4158,8 @@
   </sheetPr>
   <dimension ref="A1:K197"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A106" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G119" activeCellId="0" pane="topLeft" sqref="G119"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A158" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E166" activeCellId="0" pane="topLeft" sqref="E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9617,7 +9620,7 @@
         <v>735</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>32</v>
+        <v>736</v>
       </c>
       <c r="E172" s="8" t="n">
         <v>0</v>
@@ -9632,24 +9635,24 @@
         <v>480</v>
       </c>
       <c r="I172" s="5" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="J172" s="10" t="n">
         <v>0</v>
       </c>
       <c r="K172" s="5" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="173">
       <c r="A173" s="9" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B173" s="9" t="s">
         <v>661</v>
       </c>
       <c r="C173" s="21" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="D173" s="9" t="s">
         <v>39</v>
@@ -9667,24 +9670,24 @@
         <v>480</v>
       </c>
       <c r="I173" s="9" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="J173" s="23" t="n">
         <v>0</v>
       </c>
       <c r="K173" s="9" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="174">
       <c r="A174" s="5" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="C174" s="7" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="D174" s="5" t="s">
         <v>172</v>
@@ -9696,10 +9699,10 @@
         <v>40</v>
       </c>
       <c r="G174" s="5" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H174" s="9" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="I174" s="5" t="s">
         <v>714</v>
@@ -9708,18 +9711,18 @@
         <v>0</v>
       </c>
       <c r="K174" s="9" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="175">
       <c r="A175" s="25" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="C175" s="30" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="D175" s="25" t="s">
         <v>573</v>
@@ -9734,7 +9737,7 @@
         <v>712</v>
       </c>
       <c r="H175" s="5" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="I175" s="25" t="s">
         <v>714</v>
@@ -9743,18 +9746,18 @@
         <v>0</v>
       </c>
       <c r="K175" s="9" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="176">
       <c r="A176" s="25" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C176" s="30" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="D176" s="25" t="s">
         <v>64</v>
@@ -9766,10 +9769,10 @@
         <v>155</v>
       </c>
       <c r="G176" s="25" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="H176" s="9" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="I176" s="25" t="s">
         <v>714</v>
@@ -9778,18 +9781,18 @@
         <v>0</v>
       </c>
       <c r="K176" s="9" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="177">
       <c r="A177" s="25" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B177" s="25" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C177" s="35" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="D177" s="25" t="s">
         <v>64</v>
@@ -9804,7 +9807,7 @@
         <v>731</v>
       </c>
       <c r="H177" s="9" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="I177" s="25" t="s">
         <v>714</v>
@@ -9813,18 +9816,18 @@
         <v>0</v>
       </c>
       <c r="K177" s="9" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="178">
       <c r="A178" s="9" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B178" s="6" t="n">
         <v>16</v>
       </c>
       <c r="C178" s="24" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="D178" s="5" t="s">
         <v>64</v>
@@ -9842,24 +9845,24 @@
         <v>480</v>
       </c>
       <c r="I178" s="5" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="J178" s="29" t="n">
         <v>0</v>
       </c>
       <c r="K178" s="5" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="179">
       <c r="A179" s="9" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B179" s="26" t="n">
         <v>17</v>
       </c>
       <c r="C179" s="36" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="D179" s="25" t="s">
         <v>64</v>
@@ -9877,24 +9880,24 @@
         <v>480</v>
       </c>
       <c r="I179" s="25" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="J179" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K179" s="5" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="180">
       <c r="A180" s="25" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C180" s="30" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="D180" s="25" t="s">
         <v>172</v>
@@ -9906,10 +9909,10 @@
         <v>59</v>
       </c>
       <c r="G180" s="25" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H180" s="9" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="I180" s="25" t="s">
         <v>714</v>
@@ -9918,18 +9921,18 @@
         <v>0</v>
       </c>
       <c r="K180" s="9" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="181">
       <c r="A181" s="16" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B181" s="16" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C181" s="37" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D181" s="16" t="s">
         <v>473</v>
@@ -9941,10 +9944,10 @@
         <v>109</v>
       </c>
       <c r="G181" s="16" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="H181" s="11" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="I181" s="16" t="s">
         <v>714</v>
@@ -9953,12 +9956,12 @@
         <v>0</v>
       </c>
       <c r="K181" s="11" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="182">
       <c r="A182" s="3" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
@@ -9973,13 +9976,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="183">
       <c r="A183" s="5" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="D183" s="5" t="s">
         <v>64</v>
@@ -9997,24 +10000,24 @@
         <v>480</v>
       </c>
       <c r="I183" s="9" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="J183" s="10" t="n">
         <v>0</v>
       </c>
       <c r="K183" s="5" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="184">
       <c r="A184" s="5" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="D184" s="5" t="s">
         <v>32</v>
@@ -10029,27 +10032,27 @@
         <v>480</v>
       </c>
       <c r="H184" s="5" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="I184" s="9" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="J184" s="10" t="n">
         <v>0</v>
       </c>
       <c r="K184" s="5" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="185">
       <c r="A185" s="9" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B185" s="9" t="s">
         <v>661</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>485</v>
@@ -10064,7 +10067,7 @@
         <v>480</v>
       </c>
       <c r="H185" s="9" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="I185" s="9" t="s">
         <v>661</v>
@@ -10073,7 +10076,7 @@
         <v>0</v>
       </c>
       <c r="K185" s="9" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="186">
@@ -10113,7 +10116,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="187">
       <c r="A187" s="9" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B187" s="9" t="s">
         <v>661</v>
@@ -10137,18 +10140,18 @@
         <v>480</v>
       </c>
       <c r="I187" s="9" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="J187" s="32" t="n">
         <v>0</v>
       </c>
       <c r="K187" s="9" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="188">
       <c r="A188" s="5" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B188" s="5" t="s">
         <v>573</v>
@@ -10172,18 +10175,18 @@
         <v>480</v>
       </c>
       <c r="I188" s="5" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="J188" s="29" t="n">
         <v>0</v>
       </c>
       <c r="K188" s="5" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="189">
       <c r="A189" s="3" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
@@ -10211,13 +10214,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="191">
       <c r="A191" s="5" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B191" s="5" t="s">
         <v>661</v>
       </c>
       <c r="C191" s="24" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D191" s="5" t="s">
         <v>172</v>
@@ -10235,24 +10238,24 @@
         <v>480</v>
       </c>
       <c r="I191" s="9" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="J191" s="10" t="n">
         <v>0</v>
       </c>
       <c r="K191" s="5" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="192">
       <c r="A192" s="5" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="B192" s="5" t="s">
         <v>661</v>
       </c>
       <c r="C192" s="21" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="D192" s="5" t="s">
         <v>485</v>
@@ -10261,7 +10264,7 @@
         <v>1</v>
       </c>
       <c r="F192" s="9" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="G192" s="5" t="s">
         <v>480</v>
@@ -10270,24 +10273,24 @@
         <v>480</v>
       </c>
       <c r="I192" s="5" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="J192" s="29" t="n">
         <v>0</v>
       </c>
       <c r="K192" s="5" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="193">
       <c r="A193" s="9" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D193" s="9" t="s">
         <v>485</v>
@@ -10296,7 +10299,7 @@
         <v>0</v>
       </c>
       <c r="F193" s="9" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="G193" s="9" t="s">
         <v>480</v>
@@ -10305,24 +10308,24 @@
         <v>480</v>
       </c>
       <c r="I193" s="9" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="J193" s="32" t="n">
         <v>0</v>
       </c>
       <c r="K193" s="9" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="194">
       <c r="A194" s="9" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C194" s="9" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="D194" s="9" t="s">
         <v>485</v>
@@ -10331,7 +10334,7 @@
         <v>0</v>
       </c>
       <c r="F194" s="9" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="G194" s="9" t="s">
         <v>480</v>
@@ -10340,24 +10343,24 @@
         <v>480</v>
       </c>
       <c r="I194" s="9" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="J194" s="32" t="n">
         <v>0</v>
       </c>
       <c r="K194" s="9" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="195">
       <c r="A195" s="7" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B195" s="9" t="s">
         <v>661</v>
       </c>
       <c r="C195" s="7" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>64</v>
@@ -10375,18 +10378,18 @@
         <v>480</v>
       </c>
       <c r="I195" s="9" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="J195" s="23" t="n">
         <v>0</v>
       </c>
       <c r="K195" s="9" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="196">
       <c r="A196" s="38" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B196" s="38"/>
       <c r="C196" s="38"/>
@@ -10401,7 +10404,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="197">
       <c r="A197" s="11" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B197" s="11"/>
       <c r="C197" s="11"/>

</xml_diff>

<commit_message>
Some fixes to units.json.
</commit_message>
<xml_diff>
--- a/sits/msit_gorns.xlsx
+++ b/sits/msit_gorns.xlsx
@@ -1654,7 +1654,7 @@
   </si>
   <si>
     <t>From BD: 1
-From DD or DE: 2‡</t>
+From DD/DE: 2‡</t>
   </si>
   <si>
     <t>For BD: 5</t>
@@ -4158,8 +4158,8 @@
   </sheetPr>
   <dimension ref="A1:K197"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A167" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H171" activeCellId="0" pane="topLeft" sqref="H171"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A68" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="H87" activeCellId="0" pane="topLeft" sqref="H87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>